<commit_message>
Loaded Updated documents and Updated Scrum jorunal
</commit_message>
<xml_diff>
--- a/Design/Work Allocation.xlsx
+++ b/Design/Work Allocation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Work Allocation</t>
   </si>
@@ -55,6 +55,30 @@
   </si>
   <si>
     <t>Coding for Sprint 2</t>
+  </si>
+  <si>
+    <t>Refactored Host App</t>
+  </si>
+  <si>
+    <t>Wrote Two Extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dale </t>
+  </si>
+  <si>
+    <t>Hooked up extensions and host app</t>
+  </si>
+  <si>
+    <t>Module Decomp Diagram 2.0</t>
+  </si>
+  <si>
+    <t>Dependency Diagram 2.0</t>
+  </si>
+  <si>
+    <t>class Diagram 2.0</t>
+  </si>
+  <si>
+    <t>Startup 2.0</t>
   </si>
 </sst>
 </file>
@@ -396,20 +420,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -417,7 +441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -425,7 +449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -433,7 +457,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -441,7 +465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -449,7 +473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -457,7 +481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -465,20 +489,69 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>